<commit_message>
Solution to the leetcode array square and sort problem uploaded
</commit_message>
<xml_diff>
--- a/Interview prepration Sheet.xlsx
+++ b/Interview prepration Sheet.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="261">
   <si>
     <t>Arrays</t>
   </si>
@@ -483,15 +486,19 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
         <color rgb="FF1155CC"/>
-        <u/>
+        <rFont val="Arial"/>
       </rPr>
       <t>https://leetcode.com/problems/binary-tree-inorder-traversal/</t>
     </r>
     <r>
       <rPr>
+        <u/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
-        <u/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">   (USING STACK TOO)</t>
     </r>
@@ -804,55 +811,86 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/reverse-nodes-in-k-group/</t>
+  </si>
+  <si>
+    <t>Solution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="13">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -861,82 +899,69 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1126,1892 +1151,1899 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B1:C435"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="114.29"/>
-    <col customWidth="1" min="3" max="3" width="62.43"/>
+    <col min="2" max="2" width="114.28515625" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="2:3">
       <c r="B1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="2:3">
       <c r="B2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="2:3">
       <c r="B3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="2:3">
       <c r="B4" s="3"/>
     </row>
-    <row r="5">
+    <row r="5" spans="2:3">
       <c r="B5" s="3"/>
     </row>
-    <row r="6">
+    <row r="6" spans="2:3">
       <c r="B6" s="3"/>
     </row>
-    <row r="8">
+    <row r="8" spans="2:3">
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9">
+      <c r="C8" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="2:3">
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="7"/>
     </row>
-    <row r="11">
+    <row r="11" spans="2:3">
       <c r="B11" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="2:3">
       <c r="B12" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="7"/>
     </row>
-    <row r="13">
+    <row r="13" spans="2:3">
       <c r="B13" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="7"/>
     </row>
-    <row r="14">
+    <row r="14" spans="2:3">
       <c r="B14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="7"/>
     </row>
-    <row r="15">
+    <row r="15" spans="2:3">
       <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="7"/>
     </row>
-    <row r="16">
+    <row r="16" spans="2:3">
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="7"/>
     </row>
-    <row r="17">
+    <row r="17" spans="2:3">
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="7"/>
     </row>
-    <row r="18">
+    <row r="18" spans="2:3">
       <c r="B18" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="7"/>
     </row>
-    <row r="19">
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="2:3">
+      <c r="B19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20">
+      <c r="C19" s="18"/>
+    </row>
+    <row r="20" spans="2:3">
       <c r="B20" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="7"/>
     </row>
-    <row r="21">
+    <row r="21" spans="2:3">
       <c r="B21" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="7"/>
     </row>
-    <row r="23">
+    <row r="23" spans="2:3">
       <c r="B23" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="2:3">
       <c r="B24" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7"/>
     </row>
-    <row r="25">
+    <row r="25" spans="2:3">
       <c r="B25" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="7"/>
     </row>
-    <row r="26">
+    <row r="26" spans="2:3">
       <c r="B26" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="2:3">
       <c r="B27" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="7"/>
     </row>
-    <row r="28">
+    <row r="28" spans="2:3">
       <c r="B28" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="7"/>
     </row>
-    <row r="29">
+    <row r="29" spans="2:3">
       <c r="B29" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="2:3">
       <c r="B30" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="2:3">
       <c r="B31" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="2:3">
       <c r="B32" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="2:3">
       <c r="B33" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="2:3">
       <c r="B34" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="2:3">
       <c r="B35" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="2:3">
       <c r="B36" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="2:3">
       <c r="B37" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C37" s="7"/>
     </row>
-    <row r="38">
+    <row r="38" spans="2:3">
       <c r="B38" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="2:3">
       <c r="B39" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="2:3">
       <c r="B40" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="2:3">
       <c r="B41" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="2:3">
       <c r="B42" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="2:3">
       <c r="B43" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="2:3">
       <c r="B44" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="2:3">
       <c r="B45" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="2:3">
       <c r="B46" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="2:3">
       <c r="B47" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="2:3">
       <c r="B48" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="2:3">
       <c r="B49" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="2:3">
       <c r="B51" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="2:3">
       <c r="B52" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="2:3">
       <c r="B53" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="2:3">
       <c r="B54" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="2:3">
       <c r="B55" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C55" s="7"/>
     </row>
-    <row r="56">
+    <row r="56" spans="2:3">
       <c r="B56" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="2:3">
       <c r="B58" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="2:3">
       <c r="B59" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="2:3">
       <c r="B60" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="2:3">
       <c r="B61" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="2:3">
       <c r="B62" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C62" s="7"/>
     </row>
-    <row r="63">
+    <row r="63" spans="2:3">
       <c r="B63" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="2:3">
       <c r="B65" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="2:3">
       <c r="B66" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C66" s="7"/>
     </row>
-    <row r="67">
+    <row r="67" spans="2:3">
       <c r="B67" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C67" s="7"/>
     </row>
-    <row r="68">
+    <row r="68" spans="2:3">
       <c r="B68" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="2:3">
       <c r="B69" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="2:3">
       <c r="B70" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="2:3">
       <c r="B71" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="2:3">
       <c r="B72" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="2:3">
       <c r="B73" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="2:3">
       <c r="B74" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C74" s="7"/>
     </row>
-    <row r="75">
+    <row r="75" spans="2:3">
       <c r="B75" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="2:3">
       <c r="B76" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="2:3">
       <c r="B77" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="2:3">
       <c r="B78" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="2:3">
       <c r="B79" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="2:3">
       <c r="B80" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="2:3">
       <c r="B81" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="2:3">
       <c r="B83" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="2:3">
       <c r="B84" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="2:3">
       <c r="B85" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="2:3">
       <c r="B86" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="2:3">
       <c r="B87" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="2:3">
       <c r="B88" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="2:3">
       <c r="B89" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="2:3">
       <c r="B90" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="2:3">
       <c r="B91" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="2:3">
       <c r="B92" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C92" s="7"/>
     </row>
-    <row r="93">
+    <row r="93" spans="2:3">
       <c r="B93" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="2:3">
       <c r="B94" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="2:3">
       <c r="B95" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="2:3">
       <c r="B96" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="2:2">
       <c r="B97" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="2:2">
       <c r="B98" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="2:2">
       <c r="B100" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="2:2">
       <c r="B101" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="2:2">
       <c r="B102" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="2:2">
       <c r="B103" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="2:2">
       <c r="B104" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="2:2">
       <c r="B105" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="2:2">
       <c r="B106" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="2:2">
       <c r="B108" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="2:2">
       <c r="B109" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="2:2">
       <c r="B110" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="2:2">
       <c r="B111" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="2:3">
       <c r="B113" s="8" t="s">
         <v>92</v>
       </c>
       <c r="C113" s="7"/>
     </row>
-    <row r="114">
+    <row r="114" spans="2:3">
       <c r="B114" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="2:3">
       <c r="B115" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="2:3">
       <c r="B116" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="2:3">
       <c r="B117" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="2:3">
       <c r="B118" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="2:3">
       <c r="B119" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="2:3">
       <c r="B121" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="2:3">
       <c r="B122" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="2:3">
       <c r="B123" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="2:3">
       <c r="B124" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="2:3">
       <c r="B125" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="2:3">
       <c r="B126" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="2:3">
       <c r="B127" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="2:3">
       <c r="B128" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="2:3">
       <c r="B130" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="2:3">
       <c r="B131" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="2:3">
       <c r="B132" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="2:3">
       <c r="B133" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="2:3">
       <c r="B134" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="2:3">
       <c r="B135" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="2:3">
       <c r="B136" s="7" t="s">
         <v>111</v>
       </c>
       <c r="C136" s="7"/>
     </row>
-    <row r="137">
+    <row r="137" spans="2:3">
       <c r="B137" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="2:3">
       <c r="B138" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="2:3">
       <c r="B139" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="2:3">
       <c r="B140" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="2:3">
       <c r="B142" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="2:3">
       <c r="B143" s="7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="2:3">
       <c r="B144" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="2:2">
       <c r="B145" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="2:2">
       <c r="B146" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="2:2">
       <c r="B147" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="2:2">
       <c r="B148" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="2:2">
       <c r="B149" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="2:2">
       <c r="B151" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="2:2">
       <c r="B152" s="8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="2:2">
       <c r="B153" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="2:2">
       <c r="B154" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="2:2">
       <c r="B155" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="2:2">
       <c r="B157" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="2:2">
       <c r="B158" s="6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="2:2">
       <c r="B161" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="2:2">
       <c r="B162" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="2:2">
       <c r="B163" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="2:2">
       <c r="B164" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="2:2">
       <c r="B165" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="2:2">
       <c r="B166" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="2:2">
       <c r="B167" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="2:2">
       <c r="B168" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="2:2">
       <c r="B169" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="2:2">
       <c r="B171" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="2:2">
       <c r="B172" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="2:2">
       <c r="B173" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="2:2">
       <c r="B174" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="2:2">
       <c r="B176" s="5"/>
     </row>
-    <row r="177">
+    <row r="177" spans="2:2">
       <c r="B177" s="9"/>
     </row>
-    <row r="178">
+    <row r="178" spans="2:2">
       <c r="B178" s="7"/>
     </row>
-    <row r="179">
+    <row r="179" spans="2:2">
       <c r="B179" s="7"/>
     </row>
-    <row r="180">
+    <row r="180" spans="2:2">
       <c r="B180" s="7"/>
     </row>
-    <row r="181">
+    <row r="181" spans="2:2">
       <c r="B181" s="7"/>
     </row>
-    <row r="182">
+    <row r="182" spans="2:2">
       <c r="B182" s="7"/>
     </row>
-    <row r="183">
+    <row r="183" spans="2:2">
       <c r="B183" s="7"/>
     </row>
-    <row r="184">
+    <row r="184" spans="2:2">
       <c r="B184" s="7"/>
     </row>
-    <row r="185">
+    <row r="185" spans="2:2">
       <c r="B185" s="10"/>
     </row>
-    <row r="186">
+    <row r="186" spans="2:2">
       <c r="B186" s="7"/>
     </row>
-    <row r="188">
+    <row r="188" spans="2:2">
       <c r="B188" s="9"/>
     </row>
-    <row r="189">
+    <row r="189" spans="2:2">
       <c r="B189" s="7"/>
     </row>
-    <row r="190">
+    <row r="190" spans="2:2">
       <c r="B190" s="7"/>
     </row>
-    <row r="191">
+    <row r="191" spans="2:2">
       <c r="B191" s="7"/>
     </row>
-    <row r="192">
+    <row r="192" spans="2:2">
       <c r="B192" s="7"/>
     </row>
-    <row r="193">
+    <row r="193" spans="2:2">
       <c r="B193" s="7"/>
     </row>
-    <row r="194">
+    <row r="194" spans="2:2">
       <c r="B194" s="7"/>
     </row>
-    <row r="195">
+    <row r="195" spans="2:2">
       <c r="B195" s="7"/>
     </row>
-    <row r="196">
+    <row r="196" spans="2:2">
       <c r="B196" s="7"/>
     </row>
-    <row r="198">
+    <row r="198" spans="2:2">
       <c r="B198" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="2:2">
       <c r="B199" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="2:2">
       <c r="B200" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="2:2">
       <c r="B201" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="2:2">
       <c r="B202" s="7" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="2:2">
       <c r="B203" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="2:2">
       <c r="B204" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="2:2">
       <c r="B205" s="7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="2:2">
       <c r="B206" s="8" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="2:2">
       <c r="B207" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="2:2">
       <c r="B208" s="8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="2:2">
       <c r="B209" s="7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="2:2">
       <c r="B210" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="2:2">
       <c r="B211" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="2:2">
       <c r="B212" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="2:2">
       <c r="B213" s="8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="2:2">
       <c r="B214" s="7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="2:2">
       <c r="B215" s="7" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" spans="2:2">
       <c r="B217" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" spans="2:2">
       <c r="B218" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" spans="2:2">
       <c r="B219" s="8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" spans="2:2">
       <c r="B220" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" spans="2:2">
       <c r="B221" s="8" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" spans="2:2">
       <c r="B222" s="8" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="2:2">
       <c r="B223" s="8" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="224">
+    <row r="224" spans="2:2">
       <c r="B224" s="8" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" spans="2:2">
       <c r="B225" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="226">
+    <row r="226" spans="2:2">
       <c r="B226" s="8" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="227">
+    <row r="227" spans="2:2">
       <c r="B227" s="8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="228">
+    <row r="228" spans="2:2">
       <c r="B228" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" spans="2:2">
       <c r="B229" s="8" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="230">
+    <row r="230" spans="2:2">
       <c r="B230" s="8" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="231">
+    <row r="231" spans="2:2">
       <c r="B231" s="8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="232">
+    <row r="232" spans="2:2">
       <c r="B232" s="8" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="233">
+    <row r="233" spans="2:2">
       <c r="B233" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="234">
+    <row r="234" spans="2:2">
       <c r="B234" s="8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="235">
+    <row r="235" spans="2:2">
       <c r="B235" s="8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="237">
+    <row r="237" spans="2:2">
       <c r="B237" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="238">
+    <row r="238" spans="2:2">
       <c r="B238" s="8" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="239">
+    <row r="239" spans="2:2">
       <c r="B239" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="240">
+    <row r="240" spans="2:2">
       <c r="B240" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="241">
+    <row r="241" spans="2:2">
       <c r="B241" s="8" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="242">
+    <row r="242" spans="2:2">
       <c r="B242" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="243">
+    <row r="243" spans="2:2">
       <c r="B243" s="8" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="244">
+    <row r="244" spans="2:2">
       <c r="B244" s="8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="246">
+    <row r="246" spans="2:2">
       <c r="B246" s="5"/>
     </row>
-    <row r="247">
+    <row r="247" spans="2:2">
       <c r="B247" s="9"/>
     </row>
-    <row r="250">
+    <row r="250" spans="2:2">
       <c r="B250" s="11"/>
     </row>
-    <row r="251">
+    <row r="251" spans="2:2">
       <c r="B251" s="9"/>
     </row>
-    <row r="255">
+    <row r="255" spans="2:2">
       <c r="B255" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="256">
+    <row r="256" spans="2:2">
       <c r="B256" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="257">
+    <row r="257" spans="2:2">
       <c r="B257" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="258">
+    <row r="258" spans="2:2">
       <c r="B258" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="259">
+    <row r="259" spans="2:2">
       <c r="B259" s="8" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="260">
+    <row r="260" spans="2:2">
       <c r="B260" s="8" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="262">
+    <row r="262" spans="2:2">
       <c r="B262" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="263">
+    <row r="263" spans="2:2">
       <c r="B263" s="8" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="264">
+    <row r="264" spans="2:2">
       <c r="B264" s="8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="265">
+    <row r="265" spans="2:2">
       <c r="B265" s="8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="266">
+    <row r="266" spans="2:2">
       <c r="B266" s="8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="267">
+    <row r="267" spans="2:2">
       <c r="B267" s="8" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="268">
+    <row r="268" spans="2:2">
       <c r="B268" s="8" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="269">
+    <row r="269" spans="2:2">
       <c r="B269" s="8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="270">
+    <row r="270" spans="2:2">
       <c r="B270" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="271">
+    <row r="271" spans="2:2">
       <c r="B271" s="8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="273">
+    <row r="273" spans="2:2">
       <c r="B273" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="274">
+    <row r="274" spans="2:2">
       <c r="B274" s="8" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="275">
+    <row r="275" spans="2:2">
       <c r="B275" s="8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="276">
+    <row r="276" spans="2:2">
       <c r="B276" s="8" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="277">
+    <row r="277" spans="2:2">
       <c r="B277" s="8" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="278">
+    <row r="278" spans="2:2">
       <c r="B278" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="280">
+    <row r="280" spans="2:2">
       <c r="B280" s="5"/>
     </row>
-    <row r="281">
+    <row r="281" spans="2:2">
       <c r="B281" s="9"/>
     </row>
-    <row r="286">
+    <row r="286" spans="2:2">
       <c r="B286" s="7"/>
     </row>
-    <row r="288">
+    <row r="288" spans="2:2">
       <c r="B288" s="9"/>
     </row>
-    <row r="294">
+    <row r="294" spans="2:2">
       <c r="B294" s="5"/>
     </row>
-    <row r="295">
+    <row r="295" spans="2:2">
       <c r="B295" s="9"/>
     </row>
-    <row r="302">
+    <row r="302" spans="2:2">
       <c r="B302" s="5"/>
     </row>
-    <row r="303">
+    <row r="303" spans="2:2">
       <c r="B303" s="9"/>
     </row>
-    <row r="311">
+    <row r="311" spans="2:3">
       <c r="B311" s="9"/>
     </row>
-    <row r="312">
+    <row r="312" spans="2:3">
       <c r="B312" s="7"/>
     </row>
-    <row r="317">
+    <row r="317" spans="2:3">
       <c r="B317" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="318">
+    <row r="318" spans="2:3">
       <c r="B318" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="319">
+    <row r="319" spans="2:3">
       <c r="B319" s="8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="320">
+    <row r="320" spans="2:3">
       <c r="B320" s="8" t="s">
         <v>203</v>
       </c>
       <c r="C320" s="7"/>
     </row>
-    <row r="321">
+    <row r="321" spans="2:3">
       <c r="B321" s="8" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="322">
+    <row r="322" spans="2:3">
       <c r="B322" s="7" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="323">
+    <row r="323" spans="2:3">
       <c r="B323" s="12" t="s">
         <v>206</v>
       </c>
       <c r="C323" s="10"/>
     </row>
-    <row r="324">
+    <row r="324" spans="2:3">
       <c r="B324" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="326">
+    <row r="326" spans="2:3">
       <c r="B326" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="327">
+    <row r="327" spans="2:3">
       <c r="B327" s="7" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="328">
+    <row r="328" spans="2:3">
       <c r="B328" s="8" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="329">
+    <row r="329" spans="2:3">
       <c r="B329" s="8" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="330">
+    <row r="330" spans="2:3">
       <c r="B330" s="8" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="331">
+    <row r="331" spans="2:3">
       <c r="B331" s="7" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="332">
+    <row r="332" spans="2:3">
       <c r="B332" s="8" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="333">
+    <row r="333" spans="2:3">
       <c r="B333" s="7" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="335">
+    <row r="335" spans="2:3">
       <c r="B335" s="5"/>
     </row>
-    <row r="336">
+    <row r="336" spans="2:3">
       <c r="B336" s="9"/>
     </row>
-    <row r="337">
+    <row r="337" spans="2:2">
       <c r="B337" s="7"/>
     </row>
-    <row r="342">
+    <row r="342" spans="2:2">
       <c r="B342" s="7"/>
     </row>
-    <row r="345">
+    <row r="345" spans="2:2">
       <c r="B345" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="346">
+    <row r="346" spans="2:2">
       <c r="B346" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="347">
+    <row r="347" spans="2:2">
       <c r="B347" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="348">
+    <row r="348" spans="2:2">
       <c r="B348" s="8" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="349">
+    <row r="349" spans="2:2">
       <c r="B349" s="13"/>
     </row>
-    <row r="350">
+    <row r="350" spans="2:2">
       <c r="B350" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="351">
+    <row r="351" spans="2:2">
       <c r="B351" s="8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="352">
+    <row r="352" spans="2:2">
       <c r="B352" s="8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="353">
+    <row r="353" spans="2:2">
       <c r="B353" s="8" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="354">
+    <row r="354" spans="2:2">
       <c r="B354" s="8" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="355">
+    <row r="355" spans="2:2">
       <c r="B355" s="8" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="356">
+    <row r="356" spans="2:2">
       <c r="B356" s="8" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="357">
+    <row r="357" spans="2:2">
       <c r="B357" s="8" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="358">
+    <row r="358" spans="2:2">
       <c r="B358" s="8" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="359">
+    <row r="359" spans="2:2">
       <c r="B359" s="8" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="360">
+    <row r="360" spans="2:2">
       <c r="B360" s="8" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="361">
+    <row r="361" spans="2:2">
       <c r="B361" s="8" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="362">
+    <row r="362" spans="2:2">
       <c r="B362" s="7" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="363">
+    <row r="363" spans="2:2">
       <c r="B363" s="8" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="364">
+    <row r="364" spans="2:2">
       <c r="B364" s="8" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="366">
+    <row r="366" spans="2:2">
       <c r="B366" s="5"/>
     </row>
-    <row r="369">
+    <row r="369" spans="2:2">
       <c r="B369" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="370">
+    <row r="370" spans="2:2">
       <c r="B370" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="371">
+    <row r="371" spans="2:2">
       <c r="B371" s="15" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="372">
+    <row r="372" spans="2:2">
       <c r="B372" s="16" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="373">
+    <row r="373" spans="2:2">
       <c r="B373" s="7" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="374">
+    <row r="374" spans="2:2">
       <c r="B374" s="7" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="375">
+    <row r="375" spans="2:2">
       <c r="B375" s="7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="376">
+    <row r="376" spans="2:2">
       <c r="B376" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="377">
+    <row r="377" spans="2:2">
       <c r="B377" s="7" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="378">
+    <row r="378" spans="2:2">
       <c r="B378" s="7" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="379">
+    <row r="379" spans="2:2">
       <c r="B379" s="7" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="380">
+    <row r="380" spans="2:2">
       <c r="B380" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="381">
+    <row r="381" spans="2:2">
       <c r="B381" s="7" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="382">
+    <row r="382" spans="2:2">
       <c r="B382" s="7" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="384">
+    <row r="384" spans="2:2">
       <c r="B384" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="385">
+    <row r="385" spans="2:2">
       <c r="B385" s="8" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="386">
+    <row r="386" spans="2:2">
       <c r="B386" s="8" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="387">
+    <row r="387" spans="2:2">
       <c r="B387" s="8" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="388">
+    <row r="388" spans="2:2">
       <c r="B388" s="8" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="389">
+    <row r="389" spans="2:2">
       <c r="B389" s="7" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="390">
+    <row r="390" spans="2:2">
       <c r="B390" s="7" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="391">
+    <row r="391" spans="2:2">
       <c r="B391" s="8" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="392">
+    <row r="392" spans="2:2">
       <c r="B392" s="7" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="393">
+    <row r="393" spans="2:2">
       <c r="B393" s="8" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="394">
+    <row r="394" spans="2:2">
       <c r="B394" s="8" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="395">
+    <row r="395" spans="2:2">
       <c r="B395" s="8" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="396">
+    <row r="396" spans="2:2">
       <c r="B396" s="8" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="397">
+    <row r="397" spans="2:2">
       <c r="B397" s="8" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="399">
+    <row r="399" spans="2:2">
       <c r="B399" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="400">
+    <row r="400" spans="2:2">
       <c r="B400" s="7" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="401">
+    <row r="401" spans="2:2">
       <c r="B401" s="8" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="403">
+    <row r="403" spans="2:2">
       <c r="B403" s="5"/>
     </row>
-    <row r="404">
+    <row r="404" spans="2:2">
       <c r="B404" s="9"/>
     </row>
-    <row r="414">
+    <row r="414" spans="2:2">
       <c r="B414" s="9"/>
     </row>
-    <row r="419">
+    <row r="419" spans="2:2">
       <c r="B419" s="7"/>
     </row>
-    <row r="425">
+    <row r="425" spans="2:2">
       <c r="B425" s="5"/>
     </row>
-    <row r="426">
+    <row r="426" spans="2:2">
       <c r="B426" s="9"/>
     </row>
-    <row r="430">
+    <row r="430" spans="2:2">
       <c r="B430" s="17"/>
     </row>
-    <row r="431">
+    <row r="431" spans="2:2">
       <c r="B431" s="6"/>
     </row>
-    <row r="432">
+    <row r="432" spans="2:2">
       <c r="B432" s="5"/>
     </row>
-    <row r="433">
+    <row r="433" spans="2:2">
       <c r="B433" s="7"/>
     </row>
-    <row r="434">
+    <row r="434" spans="2:2">
       <c r="B434" s="5"/>
     </row>
-    <row r="435">
+    <row r="435" spans="2:2">
       <c r="B435" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B10"/>
-    <hyperlink r:id="rId2" ref="B11"/>
-    <hyperlink r:id="rId3" ref="B12"/>
-    <hyperlink r:id="rId4" ref="B13"/>
-    <hyperlink r:id="rId5" ref="B14"/>
-    <hyperlink r:id="rId6" ref="B15"/>
-    <hyperlink r:id="rId7" ref="B16"/>
-    <hyperlink r:id="rId8" ref="B17"/>
-    <hyperlink r:id="rId9" ref="B18"/>
-    <hyperlink r:id="rId10" ref="B19"/>
-    <hyperlink r:id="rId11" ref="B20"/>
-    <hyperlink r:id="rId12" ref="B21"/>
-    <hyperlink r:id="rId13" ref="B24"/>
-    <hyperlink r:id="rId14" ref="B25"/>
-    <hyperlink r:id="rId15" ref="B26"/>
-    <hyperlink r:id="rId16" ref="B27"/>
-    <hyperlink r:id="rId17" ref="B28"/>
-    <hyperlink r:id="rId18" ref="B29"/>
-    <hyperlink r:id="rId19" ref="B30"/>
-    <hyperlink r:id="rId20" ref="B31"/>
-    <hyperlink r:id="rId21" ref="B32"/>
-    <hyperlink r:id="rId22" ref="B33"/>
-    <hyperlink r:id="rId23" ref="B34"/>
-    <hyperlink r:id="rId24" ref="B35"/>
-    <hyperlink r:id="rId25" ref="B36"/>
-    <hyperlink r:id="rId26" ref="B37"/>
-    <hyperlink r:id="rId27" ref="B38"/>
-    <hyperlink r:id="rId28" ref="B39"/>
-    <hyperlink r:id="rId29" ref="B40"/>
-    <hyperlink r:id="rId30" ref="B41"/>
-    <hyperlink r:id="rId31" ref="B42"/>
-    <hyperlink r:id="rId32" ref="B43"/>
-    <hyperlink r:id="rId33" ref="B44"/>
-    <hyperlink r:id="rId34" ref="B45"/>
-    <hyperlink r:id="rId35" ref="B46"/>
-    <hyperlink r:id="rId36" ref="B47"/>
-    <hyperlink r:id="rId37" ref="B48"/>
-    <hyperlink r:id="rId38" ref="B49"/>
-    <hyperlink r:id="rId39" ref="B52"/>
-    <hyperlink r:id="rId40" ref="B53"/>
-    <hyperlink r:id="rId41" ref="B54"/>
-    <hyperlink r:id="rId42" ref="B55"/>
-    <hyperlink r:id="rId43" ref="B56"/>
-    <hyperlink r:id="rId44" ref="B60"/>
-    <hyperlink r:id="rId45" ref="B61"/>
-    <hyperlink r:id="rId46" ref="B62"/>
-    <hyperlink r:id="rId47" ref="B63"/>
-    <hyperlink r:id="rId48" ref="B66"/>
-    <hyperlink r:id="rId49" ref="B67"/>
-    <hyperlink r:id="rId50" ref="B68"/>
-    <hyperlink r:id="rId51" ref="B69"/>
-    <hyperlink r:id="rId52" ref="B70"/>
-    <hyperlink r:id="rId53" ref="B71"/>
-    <hyperlink r:id="rId54" ref="B72"/>
-    <hyperlink r:id="rId55" ref="B73"/>
-    <hyperlink r:id="rId56" ref="B74"/>
-    <hyperlink r:id="rId57" ref="B75"/>
-    <hyperlink r:id="rId58" ref="B76"/>
-    <hyperlink r:id="rId59" ref="B77"/>
-    <hyperlink r:id="rId60" ref="B78"/>
-    <hyperlink r:id="rId61" ref="B79"/>
-    <hyperlink r:id="rId62" ref="B80"/>
-    <hyperlink r:id="rId63" ref="B81"/>
-    <hyperlink r:id="rId64" ref="B84"/>
-    <hyperlink r:id="rId65" ref="B85"/>
-    <hyperlink r:id="rId66" ref="B86"/>
-    <hyperlink r:id="rId67" ref="B87"/>
-    <hyperlink r:id="rId68" ref="B88"/>
-    <hyperlink r:id="rId69" ref="B89"/>
-    <hyperlink r:id="rId70" ref="B90"/>
-    <hyperlink r:id="rId71" ref="B91"/>
-    <hyperlink r:id="rId72" ref="B92"/>
-    <hyperlink r:id="rId73" ref="B93"/>
-    <hyperlink r:id="rId74" ref="B94"/>
-    <hyperlink r:id="rId75" ref="B95"/>
-    <hyperlink r:id="rId76" ref="B96"/>
-    <hyperlink r:id="rId77" ref="B97"/>
-    <hyperlink r:id="rId78" ref="B98"/>
-    <hyperlink r:id="rId79" ref="B102"/>
-    <hyperlink r:id="rId80" ref="B103"/>
-    <hyperlink r:id="rId81" ref="B104"/>
-    <hyperlink r:id="rId82" ref="B105"/>
-    <hyperlink r:id="rId83" ref="B106"/>
-    <hyperlink r:id="rId84" ref="B109"/>
-    <hyperlink r:id="rId85" ref="B110"/>
-    <hyperlink r:id="rId86" ref="B111"/>
-    <hyperlink r:id="rId87" ref="B113"/>
-    <hyperlink r:id="rId88" ref="B114"/>
-    <hyperlink r:id="rId89" ref="B115"/>
-    <hyperlink r:id="rId90" ref="B116"/>
-    <hyperlink r:id="rId91" ref="B117"/>
-    <hyperlink r:id="rId92" ref="B118"/>
-    <hyperlink r:id="rId93" ref="B119"/>
-    <hyperlink r:id="rId94" ref="B122"/>
-    <hyperlink r:id="rId95" ref="B123"/>
-    <hyperlink r:id="rId96" ref="B124"/>
-    <hyperlink r:id="rId97" ref="B125"/>
-    <hyperlink r:id="rId98" ref="B126"/>
-    <hyperlink r:id="rId99" ref="B127"/>
-    <hyperlink r:id="rId100" ref="B128"/>
-    <hyperlink r:id="rId101" ref="B132"/>
-    <hyperlink r:id="rId102" ref="B133"/>
-    <hyperlink r:id="rId103" ref="B134"/>
-    <hyperlink r:id="rId104" ref="B135"/>
-    <hyperlink r:id="rId105" ref="B136"/>
-    <hyperlink r:id="rId106" ref="B137"/>
-    <hyperlink r:id="rId107" ref="B138"/>
-    <hyperlink r:id="rId108" ref="B139"/>
-    <hyperlink r:id="rId109" ref="B140"/>
-    <hyperlink r:id="rId110" ref="B143"/>
-    <hyperlink r:id="rId111" ref="B144"/>
-    <hyperlink r:id="rId112" ref="B145"/>
-    <hyperlink r:id="rId113" ref="B146"/>
-    <hyperlink r:id="rId114" ref="B147"/>
-    <hyperlink r:id="rId115" ref="B148"/>
-    <hyperlink r:id="rId116" ref="B149"/>
-    <hyperlink r:id="rId117" ref="B152"/>
-    <hyperlink r:id="rId118" ref="B153"/>
-    <hyperlink r:id="rId119" ref="B154"/>
-    <hyperlink r:id="rId120" ref="B155"/>
-    <hyperlink r:id="rId121" ref="B162"/>
-    <hyperlink r:id="rId122" ref="B163"/>
-    <hyperlink r:id="rId123" ref="B164"/>
-    <hyperlink r:id="rId124" ref="B165"/>
-    <hyperlink r:id="rId125" ref="B166"/>
-    <hyperlink r:id="rId126" ref="B167"/>
-    <hyperlink r:id="rId127" ref="B168"/>
-    <hyperlink r:id="rId128" ref="B169"/>
-    <hyperlink r:id="rId129" ref="B172"/>
-    <hyperlink r:id="rId130" ref="B173"/>
-    <hyperlink r:id="rId131" ref="B174"/>
-    <hyperlink r:id="rId132" ref="B200"/>
-    <hyperlink r:id="rId133" ref="B201"/>
-    <hyperlink r:id="rId134" ref="B202"/>
-    <hyperlink r:id="rId135" ref="B203"/>
-    <hyperlink r:id="rId136" ref="B204"/>
-    <hyperlink r:id="rId137" ref="B205"/>
-    <hyperlink r:id="rId138" ref="B206"/>
-    <hyperlink r:id="rId139" ref="B207"/>
-    <hyperlink r:id="rId140" ref="B208"/>
-    <hyperlink r:id="rId141" ref="B209"/>
-    <hyperlink r:id="rId142" ref="B210"/>
-    <hyperlink r:id="rId143" ref="B211"/>
-    <hyperlink r:id="rId144" ref="B212"/>
-    <hyperlink r:id="rId145" ref="B213"/>
-    <hyperlink r:id="rId146" ref="B214"/>
-    <hyperlink r:id="rId147" ref="B215"/>
-    <hyperlink r:id="rId148" ref="B218"/>
-    <hyperlink r:id="rId149" ref="B219"/>
-    <hyperlink r:id="rId150" ref="B220"/>
-    <hyperlink r:id="rId151" ref="B221"/>
-    <hyperlink r:id="rId152" ref="B222"/>
-    <hyperlink r:id="rId153" ref="B223"/>
-    <hyperlink r:id="rId154" ref="B224"/>
-    <hyperlink r:id="rId155" ref="B225"/>
-    <hyperlink r:id="rId156" ref="B226"/>
-    <hyperlink r:id="rId157" ref="B227"/>
-    <hyperlink r:id="rId158" ref="B228"/>
-    <hyperlink r:id="rId159" ref="B229"/>
-    <hyperlink r:id="rId160" ref="B230"/>
-    <hyperlink r:id="rId161" ref="B231"/>
-    <hyperlink r:id="rId162" ref="B232"/>
-    <hyperlink r:id="rId163" ref="B233"/>
-    <hyperlink r:id="rId164" ref="B234"/>
-    <hyperlink r:id="rId165" ref="B235"/>
-    <hyperlink r:id="rId166" ref="B238"/>
-    <hyperlink r:id="rId167" ref="B239"/>
-    <hyperlink r:id="rId168" ref="B240"/>
-    <hyperlink r:id="rId169" ref="B241"/>
-    <hyperlink r:id="rId170" ref="B242"/>
-    <hyperlink r:id="rId171" ref="B243"/>
-    <hyperlink r:id="rId172" ref="B244"/>
-    <hyperlink r:id="rId173" ref="B257"/>
-    <hyperlink r:id="rId174" ref="B258"/>
-    <hyperlink r:id="rId175" ref="B259"/>
-    <hyperlink r:id="rId176" ref="B260"/>
-    <hyperlink r:id="rId177" ref="B263"/>
-    <hyperlink r:id="rId178" ref="B264"/>
-    <hyperlink r:id="rId179" ref="B265"/>
-    <hyperlink r:id="rId180" ref="B266"/>
-    <hyperlink r:id="rId181" ref="B267"/>
-    <hyperlink r:id="rId182" ref="B268"/>
-    <hyperlink r:id="rId183" ref="B269"/>
-    <hyperlink r:id="rId184" ref="B270"/>
-    <hyperlink r:id="rId185" ref="B271"/>
-    <hyperlink r:id="rId186" ref="B274"/>
-    <hyperlink r:id="rId187" ref="B275"/>
-    <hyperlink r:id="rId188" ref="B276"/>
-    <hyperlink r:id="rId189" ref="B277"/>
-    <hyperlink r:id="rId190" ref="B278"/>
-    <hyperlink r:id="rId191" ref="B319"/>
-    <hyperlink r:id="rId192" ref="B320"/>
-    <hyperlink r:id="rId193" ref="B321"/>
-    <hyperlink r:id="rId194" ref="B322"/>
-    <hyperlink r:id="rId195" ref="B324"/>
-    <hyperlink r:id="rId196" ref="B327"/>
-    <hyperlink r:id="rId197" ref="B328"/>
-    <hyperlink r:id="rId198" ref="B329"/>
-    <hyperlink r:id="rId199" ref="B330"/>
-    <hyperlink r:id="rId200" ref="B331"/>
-    <hyperlink r:id="rId201" ref="B332"/>
-    <hyperlink r:id="rId202" ref="B333"/>
-    <hyperlink r:id="rId203" ref="B347"/>
-    <hyperlink r:id="rId204" ref="B348"/>
-    <hyperlink r:id="rId205" ref="B351"/>
-    <hyperlink r:id="rId206" ref="B352"/>
-    <hyperlink r:id="rId207" ref="B353"/>
-    <hyperlink r:id="rId208" ref="B354"/>
-    <hyperlink r:id="rId209" ref="B355"/>
-    <hyperlink r:id="rId210" ref="B356"/>
-    <hyperlink r:id="rId211" ref="B357"/>
-    <hyperlink r:id="rId212" ref="B358"/>
-    <hyperlink r:id="rId213" ref="B359"/>
-    <hyperlink r:id="rId214" ref="B360"/>
-    <hyperlink r:id="rId215" ref="B361"/>
-    <hyperlink r:id="rId216" ref="B362"/>
-    <hyperlink r:id="rId217" ref="B363"/>
-    <hyperlink r:id="rId218" ref="B364"/>
-    <hyperlink r:id="rId219" ref="B371"/>
-    <hyperlink r:id="rId220" ref="B372"/>
-    <hyperlink r:id="rId221" ref="B373"/>
-    <hyperlink r:id="rId222" ref="B374"/>
-    <hyperlink r:id="rId223" ref="B375"/>
-    <hyperlink r:id="rId224" ref="B376"/>
-    <hyperlink r:id="rId225" ref="B377"/>
-    <hyperlink r:id="rId226" ref="B378"/>
-    <hyperlink r:id="rId227" ref="B379"/>
-    <hyperlink r:id="rId228" ref="B380"/>
-    <hyperlink r:id="rId229" ref="B381"/>
-    <hyperlink r:id="rId230" ref="B382"/>
-    <hyperlink r:id="rId231" ref="B385"/>
-    <hyperlink r:id="rId232" ref="B386"/>
-    <hyperlink r:id="rId233" ref="B387"/>
-    <hyperlink r:id="rId234" ref="B388"/>
-    <hyperlink r:id="rId235" ref="B389"/>
-    <hyperlink r:id="rId236" ref="B390"/>
-    <hyperlink r:id="rId237" ref="B391"/>
-    <hyperlink r:id="rId238" ref="B392"/>
-    <hyperlink r:id="rId239" ref="B393"/>
-    <hyperlink r:id="rId240" ref="B394"/>
-    <hyperlink r:id="rId241" ref="B395"/>
-    <hyperlink r:id="rId242" ref="B396"/>
-    <hyperlink r:id="rId243" ref="B397"/>
-    <hyperlink r:id="rId244" ref="B400"/>
-    <hyperlink r:id="rId245" ref="B401"/>
+    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B12" r:id="rId3"/>
+    <hyperlink ref="B13" r:id="rId4"/>
+    <hyperlink ref="B14" r:id="rId5"/>
+    <hyperlink ref="B15" r:id="rId6"/>
+    <hyperlink ref="B16" r:id="rId7"/>
+    <hyperlink ref="B17" r:id="rId8"/>
+    <hyperlink ref="B18" r:id="rId9"/>
+    <hyperlink ref="B19" r:id="rId10"/>
+    <hyperlink ref="B20" r:id="rId11"/>
+    <hyperlink ref="B21" r:id="rId12"/>
+    <hyperlink ref="B24" r:id="rId13"/>
+    <hyperlink ref="B25" r:id="rId14"/>
+    <hyperlink ref="B26" r:id="rId15"/>
+    <hyperlink ref="B27" r:id="rId16"/>
+    <hyperlink ref="B28" r:id="rId17"/>
+    <hyperlink ref="B29" r:id="rId18"/>
+    <hyperlink ref="B30" r:id="rId19"/>
+    <hyperlink ref="B31" r:id="rId20"/>
+    <hyperlink ref="B32" r:id="rId21"/>
+    <hyperlink ref="B33" r:id="rId22"/>
+    <hyperlink ref="B34" r:id="rId23"/>
+    <hyperlink ref="B35" r:id="rId24"/>
+    <hyperlink ref="B36" r:id="rId25"/>
+    <hyperlink ref="B37" r:id="rId26"/>
+    <hyperlink ref="B38" r:id="rId27"/>
+    <hyperlink ref="B39" r:id="rId28"/>
+    <hyperlink ref="B40" r:id="rId29"/>
+    <hyperlink ref="B41" r:id="rId30"/>
+    <hyperlink ref="B42" r:id="rId31"/>
+    <hyperlink ref="B43" r:id="rId32"/>
+    <hyperlink ref="B44" r:id="rId33"/>
+    <hyperlink ref="B45" r:id="rId34"/>
+    <hyperlink ref="B46" r:id="rId35"/>
+    <hyperlink ref="B47" r:id="rId36"/>
+    <hyperlink ref="B48" r:id="rId37"/>
+    <hyperlink ref="B49" r:id="rId38"/>
+    <hyperlink ref="B52" r:id="rId39"/>
+    <hyperlink ref="B53" r:id="rId40"/>
+    <hyperlink ref="B54" r:id="rId41"/>
+    <hyperlink ref="B55" r:id="rId42"/>
+    <hyperlink ref="B56" r:id="rId43"/>
+    <hyperlink ref="B60" r:id="rId44"/>
+    <hyperlink ref="B61" r:id="rId45"/>
+    <hyperlink ref="B62" r:id="rId46"/>
+    <hyperlink ref="B63" r:id="rId47"/>
+    <hyperlink ref="B66" r:id="rId48"/>
+    <hyperlink ref="B67" r:id="rId49"/>
+    <hyperlink ref="B68" r:id="rId50"/>
+    <hyperlink ref="B69" r:id="rId51"/>
+    <hyperlink ref="B70" r:id="rId52"/>
+    <hyperlink ref="B71" r:id="rId53"/>
+    <hyperlink ref="B72" r:id="rId54"/>
+    <hyperlink ref="B73" r:id="rId55"/>
+    <hyperlink ref="B74" r:id="rId56"/>
+    <hyperlink ref="B75" r:id="rId57"/>
+    <hyperlink ref="B76" r:id="rId58"/>
+    <hyperlink ref="B77" r:id="rId59"/>
+    <hyperlink ref="B78" r:id="rId60"/>
+    <hyperlink ref="B79" r:id="rId61"/>
+    <hyperlink ref="B80" r:id="rId62"/>
+    <hyperlink ref="B81" r:id="rId63"/>
+    <hyperlink ref="B84" r:id="rId64"/>
+    <hyperlink ref="B85" r:id="rId65"/>
+    <hyperlink ref="B86" r:id="rId66"/>
+    <hyperlink ref="B87" r:id="rId67"/>
+    <hyperlink ref="B88" r:id="rId68"/>
+    <hyperlink ref="B89" r:id="rId69"/>
+    <hyperlink ref="B90" r:id="rId70"/>
+    <hyperlink ref="B91" r:id="rId71"/>
+    <hyperlink ref="B92" r:id="rId72"/>
+    <hyperlink ref="B93" r:id="rId73"/>
+    <hyperlink ref="B94" r:id="rId74"/>
+    <hyperlink ref="B95" r:id="rId75"/>
+    <hyperlink ref="B96" r:id="rId76"/>
+    <hyperlink ref="B97" r:id="rId77"/>
+    <hyperlink ref="B98" r:id="rId78"/>
+    <hyperlink ref="B102" r:id="rId79"/>
+    <hyperlink ref="B103" r:id="rId80"/>
+    <hyperlink ref="B104" r:id="rId81"/>
+    <hyperlink ref="B105" r:id="rId82"/>
+    <hyperlink ref="B106" r:id="rId83"/>
+    <hyperlink ref="B109" r:id="rId84"/>
+    <hyperlink ref="B110" r:id="rId85"/>
+    <hyperlink ref="B111" r:id="rId86"/>
+    <hyperlink ref="B113" r:id="rId87"/>
+    <hyperlink ref="B114" r:id="rId88"/>
+    <hyperlink ref="B115" r:id="rId89"/>
+    <hyperlink ref="B116" r:id="rId90"/>
+    <hyperlink ref="B117" r:id="rId91"/>
+    <hyperlink ref="B118" r:id="rId92"/>
+    <hyperlink ref="B119" r:id="rId93"/>
+    <hyperlink ref="B122" r:id="rId94"/>
+    <hyperlink ref="B123" r:id="rId95"/>
+    <hyperlink ref="B124" r:id="rId96"/>
+    <hyperlink ref="B125" r:id="rId97"/>
+    <hyperlink ref="B126" r:id="rId98"/>
+    <hyperlink ref="B127" r:id="rId99"/>
+    <hyperlink ref="B128" r:id="rId100"/>
+    <hyperlink ref="B132" r:id="rId101"/>
+    <hyperlink ref="B133" r:id="rId102"/>
+    <hyperlink ref="B134" r:id="rId103"/>
+    <hyperlink ref="B135" r:id="rId104"/>
+    <hyperlink ref="B136" r:id="rId105"/>
+    <hyperlink ref="B137" r:id="rId106"/>
+    <hyperlink ref="B138" r:id="rId107"/>
+    <hyperlink ref="B139" r:id="rId108"/>
+    <hyperlink ref="B140" r:id="rId109"/>
+    <hyperlink ref="B143" r:id="rId110"/>
+    <hyperlink ref="B144" r:id="rId111"/>
+    <hyperlink ref="B145" r:id="rId112"/>
+    <hyperlink ref="B146" r:id="rId113"/>
+    <hyperlink ref="B147" r:id="rId114"/>
+    <hyperlink ref="B148" r:id="rId115"/>
+    <hyperlink ref="B149" r:id="rId116"/>
+    <hyperlink ref="B152" r:id="rId117"/>
+    <hyperlink ref="B153" r:id="rId118"/>
+    <hyperlink ref="B154" r:id="rId119"/>
+    <hyperlink ref="B155" r:id="rId120"/>
+    <hyperlink ref="B162" r:id="rId121"/>
+    <hyperlink ref="B163" r:id="rId122"/>
+    <hyperlink ref="B164" r:id="rId123"/>
+    <hyperlink ref="B165" r:id="rId124"/>
+    <hyperlink ref="B166" r:id="rId125"/>
+    <hyperlink ref="B167" r:id="rId126"/>
+    <hyperlink ref="B168" r:id="rId127"/>
+    <hyperlink ref="B169" r:id="rId128"/>
+    <hyperlink ref="B172" r:id="rId129"/>
+    <hyperlink ref="B173" r:id="rId130"/>
+    <hyperlink ref="B174" r:id="rId131"/>
+    <hyperlink ref="B200" r:id="rId132"/>
+    <hyperlink ref="B201" r:id="rId133"/>
+    <hyperlink ref="B202" r:id="rId134"/>
+    <hyperlink ref="B203" r:id="rId135"/>
+    <hyperlink ref="B204" r:id="rId136"/>
+    <hyperlink ref="B205" r:id="rId137"/>
+    <hyperlink ref="B206" r:id="rId138"/>
+    <hyperlink ref="B207" r:id="rId139"/>
+    <hyperlink ref="B208" r:id="rId140"/>
+    <hyperlink ref="B209" r:id="rId141"/>
+    <hyperlink ref="B210" r:id="rId142"/>
+    <hyperlink ref="B211" r:id="rId143"/>
+    <hyperlink ref="B212" r:id="rId144"/>
+    <hyperlink ref="B213" r:id="rId145"/>
+    <hyperlink ref="B214" r:id="rId146"/>
+    <hyperlink ref="B215" r:id="rId147"/>
+    <hyperlink ref="B218" r:id="rId148"/>
+    <hyperlink ref="B219" r:id="rId149"/>
+    <hyperlink ref="B220" r:id="rId150"/>
+    <hyperlink ref="B221" r:id="rId151"/>
+    <hyperlink ref="B222" r:id="rId152"/>
+    <hyperlink ref="B223" r:id="rId153"/>
+    <hyperlink ref="B224" r:id="rId154"/>
+    <hyperlink ref="B225" r:id="rId155"/>
+    <hyperlink ref="B226" r:id="rId156"/>
+    <hyperlink ref="B227" r:id="rId157"/>
+    <hyperlink ref="B228" r:id="rId158"/>
+    <hyperlink ref="B229" r:id="rId159"/>
+    <hyperlink ref="B230" r:id="rId160"/>
+    <hyperlink ref="B231" r:id="rId161"/>
+    <hyperlink ref="B232" r:id="rId162"/>
+    <hyperlink ref="B233" r:id="rId163"/>
+    <hyperlink ref="B234" r:id="rId164"/>
+    <hyperlink ref="B235" r:id="rId165"/>
+    <hyperlink ref="B238" r:id="rId166"/>
+    <hyperlink ref="B239" r:id="rId167"/>
+    <hyperlink ref="B240" r:id="rId168"/>
+    <hyperlink ref="B241" r:id="rId169"/>
+    <hyperlink ref="B242" r:id="rId170"/>
+    <hyperlink ref="B243" r:id="rId171"/>
+    <hyperlink ref="B244" r:id="rId172"/>
+    <hyperlink ref="B257" r:id="rId173"/>
+    <hyperlink ref="B258" r:id="rId174"/>
+    <hyperlink ref="B259" r:id="rId175"/>
+    <hyperlink ref="B260" r:id="rId176"/>
+    <hyperlink ref="B263" r:id="rId177"/>
+    <hyperlink ref="B264" r:id="rId178"/>
+    <hyperlink ref="B265" r:id="rId179"/>
+    <hyperlink ref="B266" r:id="rId180"/>
+    <hyperlink ref="B267" r:id="rId181"/>
+    <hyperlink ref="B268" r:id="rId182"/>
+    <hyperlink ref="B269" r:id="rId183"/>
+    <hyperlink ref="B270" r:id="rId184"/>
+    <hyperlink ref="B271" r:id="rId185"/>
+    <hyperlink ref="B274" r:id="rId186"/>
+    <hyperlink ref="B275" r:id="rId187"/>
+    <hyperlink ref="B276" r:id="rId188"/>
+    <hyperlink ref="B277" r:id="rId189"/>
+    <hyperlink ref="B278" r:id="rId190"/>
+    <hyperlink ref="B319" r:id="rId191"/>
+    <hyperlink ref="B320" r:id="rId192"/>
+    <hyperlink ref="B321" r:id="rId193"/>
+    <hyperlink ref="B322" r:id="rId194"/>
+    <hyperlink ref="B324" r:id="rId195"/>
+    <hyperlink ref="B327" r:id="rId196"/>
+    <hyperlink ref="B328" r:id="rId197"/>
+    <hyperlink ref="B329" r:id="rId198"/>
+    <hyperlink ref="B330" r:id="rId199"/>
+    <hyperlink ref="B331" r:id="rId200"/>
+    <hyperlink ref="B332" r:id="rId201"/>
+    <hyperlink ref="B333" r:id="rId202"/>
+    <hyperlink ref="B347" r:id="rId203"/>
+    <hyperlink ref="B348" r:id="rId204"/>
+    <hyperlink ref="B351" r:id="rId205"/>
+    <hyperlink ref="B352" r:id="rId206"/>
+    <hyperlink ref="B353" r:id="rId207"/>
+    <hyperlink ref="B354" r:id="rId208"/>
+    <hyperlink ref="B355" r:id="rId209"/>
+    <hyperlink ref="B356" r:id="rId210"/>
+    <hyperlink ref="B357" r:id="rId211"/>
+    <hyperlink ref="B358" r:id="rId212"/>
+    <hyperlink ref="B359" r:id="rId213"/>
+    <hyperlink ref="B360" r:id="rId214"/>
+    <hyperlink ref="B361" r:id="rId215"/>
+    <hyperlink ref="B362" r:id="rId216"/>
+    <hyperlink ref="B363" r:id="rId217"/>
+    <hyperlink ref="B364" r:id="rId218"/>
+    <hyperlink ref="B371" r:id="rId219"/>
+    <hyperlink ref="B372" r:id="rId220"/>
+    <hyperlink ref="B373" r:id="rId221"/>
+    <hyperlink ref="B374" r:id="rId222"/>
+    <hyperlink ref="B375" r:id="rId223"/>
+    <hyperlink ref="B376" r:id="rId224"/>
+    <hyperlink ref="B377" r:id="rId225"/>
+    <hyperlink ref="B378" r:id="rId226"/>
+    <hyperlink ref="B379" r:id="rId227"/>
+    <hyperlink ref="B380" r:id="rId228"/>
+    <hyperlink ref="B381" r:id="rId229"/>
+    <hyperlink ref="B382" r:id="rId230"/>
+    <hyperlink ref="B385" r:id="rId231"/>
+    <hyperlink ref="B386" r:id="rId232"/>
+    <hyperlink ref="B387" r:id="rId233"/>
+    <hyperlink ref="B388" r:id="rId234"/>
+    <hyperlink ref="B389" r:id="rId235"/>
+    <hyperlink ref="B390" r:id="rId236"/>
+    <hyperlink ref="B391" r:id="rId237"/>
+    <hyperlink ref="B392" r:id="rId238"/>
+    <hyperlink ref="B393" r:id="rId239"/>
+    <hyperlink ref="B394" r:id="rId240"/>
+    <hyperlink ref="B395" r:id="rId241"/>
+    <hyperlink ref="B396" r:id="rId242"/>
+    <hyperlink ref="B397" r:id="rId243"/>
+    <hyperlink ref="B400" r:id="rId244"/>
+    <hyperlink ref="B401" r:id="rId245"/>
   </hyperlinks>
-  <drawing r:id="rId246"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>